<commit_message>
Them tt chuong sach TA
</commit_message>
<xml_diff>
--- a/DSSV/ds_20161.xlsx
+++ b/DSSV/ds_20161.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="168">
   <si>
     <t>AB</t>
   </si>
@@ -567,12 +567,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3478,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3489,9 +3490,10 @@
     <col min="1" max="1" width="4.5" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="5.125" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3505,7 +3507,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3518,8 +3520,11 @@
       <c r="D2" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="5">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3532,8 +3537,14 @@
       <c r="D3" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -3547,7 +3558,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -3561,7 +3572,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3575,7 +3586,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
@@ -3589,7 +3600,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3603,7 +3614,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14</v>
       </c>
@@ -3617,7 +3628,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>15</v>
       </c>
@@ -3631,7 +3642,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
@@ -3645,7 +3656,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
@@ -3659,7 +3670,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -3673,7 +3684,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>21</v>
       </c>
@@ -3687,7 +3698,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>25</v>
       </c>
@@ -3701,7 +3712,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Điều chỉnh tên bài và tên tệp
</commit_message>
<xml_diff>
--- a/DSSV/ds_20161.xlsx
+++ b/DSSV/ds_20161.xlsx
@@ -3479,10 +3479,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3491,9 +3491,10 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="5.125" customWidth="1"/>
     <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -3520,11 +3521,8 @@
       <c r="D2" t="s">
         <v>134</v>
       </c>
-      <c r="E2" s="5">
-        <v>42695</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -3537,14 +3535,8 @@
       <c r="D3" t="s">
         <v>136</v>
       </c>
-      <c r="E3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>5</v>
       </c>
@@ -3558,7 +3550,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>6</v>
       </c>
@@ -3572,7 +3564,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3586,7 +3578,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>11</v>
       </c>
@@ -3600,7 +3592,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>12</v>
       </c>
@@ -3614,7 +3606,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14</v>
       </c>
@@ -3628,7 +3620,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>15</v>
       </c>
@@ -3642,7 +3634,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>16</v>
       </c>
@@ -3656,7 +3648,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>18</v>
       </c>
@@ -3670,7 +3662,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20</v>
       </c>
@@ -3684,7 +3676,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>21</v>
       </c>
@@ -3698,7 +3690,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>25</v>
       </c>
@@ -3712,7 +3704,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>27</v>
       </c>
@@ -4174,7 +4166,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>43</v>
       </c>
@@ -4188,7 +4180,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>44</v>
       </c>
@@ -4202,7 +4194,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>46</v>
       </c>
@@ -4216,7 +4208,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>49</v>
       </c>
@@ -4230,7 +4222,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -4244,7 +4236,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>54</v>
       </c>
@@ -4258,7 +4250,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>55</v>
       </c>
@@ -4272,7 +4264,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
         <v>154</v>
       </c>
@@ -4280,30 +4272,39 @@
         <v>156</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
         <v>155</v>
       </c>
       <c r="D59" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="M59" s="5">
+        <v>42695</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="M60" t="s">
+        <v>132</v>
+      </c>
+      <c r="N60" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D61" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
         <v>160</v>
       </c>

</xml_diff>